<commit_message>
Added lateral-only slosh to tanker trailer. Updated Mask descriptions.
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
+++ b/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\simscape\demos\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Body\Load_Slosh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\ssvt\Libraries\Vehicle\Body\Load_Slosh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230CD7E7-B1FE-45A1-9808-5610D33CCD21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13039EB4-C7DF-4042-A612-12AB96A30988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
+    <workbookView xWindow="5676" yWindow="324" windowWidth="15660" windowHeight="7428" tabRatio="805" activeTab="3" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Slosh_3_Pend_Kumanzi" sheetId="3" r:id="rId1"/>
     <sheet name="Slosh_3_Pend_Tank" sheetId="6" r:id="rId2"/>
-    <sheet name="None" sheetId="5" r:id="rId3"/>
+    <sheet name="Tank_Cyl_Kumanzi" sheetId="7" r:id="rId3"/>
+    <sheet name="Tank_Cyl_Tank" sheetId="8" r:id="rId4"/>
+    <sheet name="None" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="36">
   <si>
     <t>Units</t>
   </si>
@@ -104,6 +106,45 @@
   </si>
   <si>
     <t>Trailer_Tank_Slosh_3_Pendulum</t>
+  </si>
+  <si>
+    <t>Tank_Cylindrical</t>
+  </si>
+  <si>
+    <t>xRefToTankCtr</t>
+  </si>
+  <si>
+    <t>Trailer_Kumanzi_Tank_Cylindrical</t>
+  </si>
+  <si>
+    <t>xRadius</t>
+  </si>
+  <si>
+    <t>(0-1)</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>Opacity</t>
+  </si>
+  <si>
+    <t>rFillHeight</t>
+  </si>
+  <si>
+    <t>dLoad</t>
+  </si>
+  <si>
+    <t>Trailer_Tank_Tank_Cylindrical</t>
   </si>
 </sst>
 </file>
@@ -130,7 +171,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +196,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -168,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -208,6 +255,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,21 +583,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -566,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -580,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -594,7 +645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -609,7 +660,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -626,12 +677,12 @@
         <v>0</v>
       </c>
       <c r="H5" s="15">
-        <f>1.5+0.2+1.25+1</f>
-        <v>3.95</v>
+        <f>1.5+0.2+1.15+0.2</f>
+        <v>3.05</v>
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -643,11 +694,11 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15">
-        <v>3</v>
+        <v>4.3</v>
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -665,7 +716,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -681,7 +732,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -697,7 +748,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -726,26 +777,26 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -765,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -779,7 +830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -793,7 +844,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -808,7 +859,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -825,12 +876,12 @@
         <v>0</v>
       </c>
       <c r="H5" s="15">
-        <f>1.5+0.2+1.25+1</f>
-        <v>3.95</v>
+        <f>1.7+0.2+1.25+0.2</f>
+        <v>3.35</v>
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -842,11 +893,11 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15">
-        <v>3</v>
+        <v>4.3</v>
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -864,7 +915,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -880,7 +931,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -896,7 +947,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -919,6 +970,466 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E446BD74-EA73-457F-AB18-532DCA18F624}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E9" sqref="E9"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="8" width="10" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="15">
+        <f>8.8-12.2/2-0.23</f>
+        <v>2.4700000000000011</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <f>2.8-0.02</f>
+        <v>2.78</v>
+      </c>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L6" s="13"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15">
+        <v>12</v>
+      </c>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="L8" s="13"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15">
+        <v>100</v>
+      </c>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="H11" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46952C8-8D44-41F6-BFC2-919868F4C529}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E9" sqref="E9"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="8" width="10" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="15">
+        <f>10-13/2</f>
+        <v>3.5</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <f>1.7+0.2+1.25</f>
+        <v>3.15</v>
+      </c>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="L6" s="13"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15">
+        <v>12.8</v>
+      </c>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="L8" s="13"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15">
+        <v>100</v>
+      </c>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="H11" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8A48EA-D7E1-42FA-B419-38DA06C02F93}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -933,18 +1444,18 @@
       <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -964,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -978,7 +1489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -992,7 +1503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Initial commit v2p1, R2018b
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
+++ b/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\ssvt\Libraries\Vehicle\Body\Load_Slosh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Body\Load_Slosh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13039EB4-C7DF-4042-A612-12AB96A30988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03FCF4B-0DAC-4509-BD98-9FBD32FED552}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5676" yWindow="324" windowWidth="15660" windowHeight="7428" tabRatio="805" activeTab="3" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="805" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Slosh_3_Pend_Kumanzi" sheetId="3" r:id="rId1"/>
@@ -578,26 +578,26 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -617,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -645,7 +645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -660,7 +660,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -682,7 +682,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -698,7 +698,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -716,7 +716,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -728,11 +728,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -748,7 +748,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -782,21 +782,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -830,7 +830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -844,7 +844,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -859,7 +859,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -897,7 +897,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -927,11 +927,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -947,7 +947,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -981,21 +981,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1156,11 +1156,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1206,26 +1206,26 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1245,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1386,11 +1386,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1444,18 +1444,18 @@
       <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1475,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Initial commit v2p1, R2019a
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
+++ b/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\ssvt\Libraries\Vehicle\Body\Load_Slosh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Body\Load_Slosh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13039EB4-C7DF-4042-A612-12AB96A30988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03FCF4B-0DAC-4509-BD98-9FBD32FED552}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5676" yWindow="324" windowWidth="15660" windowHeight="7428" tabRatio="805" activeTab="3" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="805" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Slosh_3_Pend_Kumanzi" sheetId="3" r:id="rId1"/>
@@ -578,26 +578,26 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -617,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -645,7 +645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -660,7 +660,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -682,7 +682,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -698,7 +698,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -716,7 +716,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -728,11 +728,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -748,7 +748,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -782,21 +782,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -830,7 +830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -844,7 +844,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -859,7 +859,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -897,7 +897,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -927,11 +927,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -947,7 +947,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -981,21 +981,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1156,11 +1156,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1206,26 +1206,26 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1245,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1386,11 +1386,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1444,18 +1444,18 @@
       <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1475,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Initial commit v2p1, R2019b
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
+++ b/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\ssvt\Libraries\Vehicle\Body\Load_Slosh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Body\Load_Slosh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13039EB4-C7DF-4042-A612-12AB96A30988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03FCF4B-0DAC-4509-BD98-9FBD32FED552}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5676" yWindow="324" windowWidth="15660" windowHeight="7428" tabRatio="805" activeTab="3" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="805" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Slosh_3_Pend_Kumanzi" sheetId="3" r:id="rId1"/>
@@ -578,26 +578,26 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -617,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -645,7 +645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -660,7 +660,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -682,7 +682,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -698,7 +698,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -716,7 +716,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -728,11 +728,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -748,7 +748,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -782,21 +782,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -830,7 +830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -844,7 +844,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -859,7 +859,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -897,7 +897,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -927,11 +927,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -947,7 +947,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -981,21 +981,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1156,11 +1156,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1206,26 +1206,26 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1245,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1386,11 +1386,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1444,18 +1444,18 @@
       <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1475,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Initial commit v2p1, R2020a
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
+++ b/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\ssvt\Libraries\Vehicle\Body\Load_Slosh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Body\Load_Slosh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13039EB4-C7DF-4042-A612-12AB96A30988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03FCF4B-0DAC-4509-BD98-9FBD32FED552}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5676" yWindow="324" windowWidth="15660" windowHeight="7428" tabRatio="805" activeTab="3" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="805" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Slosh_3_Pend_Kumanzi" sheetId="3" r:id="rId1"/>
@@ -578,26 +578,26 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -617,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -645,7 +645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -660,7 +660,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -682,7 +682,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -698,7 +698,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -716,7 +716,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -728,11 +728,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -748,7 +748,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -782,21 +782,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -830,7 +830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -844,7 +844,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -859,7 +859,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -897,7 +897,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -927,11 +927,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -947,7 +947,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -981,21 +981,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1156,11 +1156,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1206,26 +1206,26 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1245,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1386,11 +1386,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1444,18 +1444,18 @@
       <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1475,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Initial commit v2p1, R2020b
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
+++ b/Libraries/Vehicle/Body/Load_Slosh/sm_car_data_BodyLoad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\ssvt\Libraries\Vehicle\Body\Load_Slosh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Body\Load_Slosh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13039EB4-C7DF-4042-A612-12AB96A30988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03FCF4B-0DAC-4509-BD98-9FBD32FED552}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5676" yWindow="324" windowWidth="15660" windowHeight="7428" tabRatio="805" activeTab="3" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="805" xr2:uid="{06440896-8E0F-4240-830D-6ADD843B9DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Slosh_3_Pend_Kumanzi" sheetId="3" r:id="rId1"/>
@@ -578,26 +578,26 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -617,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -645,7 +645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -660,7 +660,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -682,7 +682,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -698,7 +698,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -716,7 +716,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -728,11 +728,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -748,7 +748,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -782,21 +782,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -830,7 +830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -844,7 +844,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -859,7 +859,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -897,7 +897,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -927,11 +927,11 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="14" t="s">
         <v>16</v>
@@ -947,7 +947,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="14" t="s">
         <v>17</v>
@@ -981,21 +981,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1156,11 +1156,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1206,26 +1206,26 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1245,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1386,11 +1386,11 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>32</v>
       </c>
@@ -1444,18 +1444,18 @@
       <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1475,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>

</xml_diff>